<commit_message>
Add zod validation on import excel
</commit_message>
<xml_diff>
--- a/example.xlsx
+++ b/example.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\wahyupranata\code\excel2json-research\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\wahyupranata\code\excel-json-research\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45303ACF-D4F9-454E-92F7-6A5D37099236}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BA0BCE6-326D-4B65-AD05-485D7C83FB17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" tabRatio="205" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2340" yWindow="2340" windowWidth="15375" windowHeight="8325" tabRatio="205" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="508" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="507" uniqueCount="117">
   <si>
     <t>First Name</t>
   </si>
@@ -368,6 +368,9 @@
   </si>
   <si>
     <t>Index</t>
+  </si>
+  <si>
+    <t>Bruh</t>
   </si>
 </sst>
 </file>
@@ -730,7 +733,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H101"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -826,7 +831,7 @@
         <v>17</v>
       </c>
       <c r="D4" t="s">
-        <v>18</v>
+        <v>116</v>
       </c>
       <c r="E4" t="s">
         <v>19</v>
@@ -1056,8 +1061,8 @@
       <c r="B13" t="s">
         <v>37</v>
       </c>
-      <c r="C13" t="s">
-        <v>38</v>
+      <c r="C13">
+        <v>12</v>
       </c>
       <c r="D13" t="s">
         <v>18</v>

</xml_diff>